<commit_message>
edited so lines are grey; numbers are bigger
</commit_message>
<xml_diff>
--- a/riskbenefit.xlsx
+++ b/riskbenefit.xlsx
@@ -252,8 +252,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.018868617032627"/>
-                  <c:y val="-0.0614118060083255"/>
+                  <c:x val="-0.0513890489298593"/>
+                  <c:y val="-0.0019638229934634"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -279,8 +279,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.0146072594584214"/>
-                  <c:y val="-0.0823354564755838"/>
+                  <c:x val="-0.0240925676973305"/>
+                  <c:y val="-0.0695966029723991"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -1151,11 +1151,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="588486440"/>
-        <c:axId val="677462872"/>
+        <c:axId val="736057048"/>
+        <c:axId val="735665432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="588486440"/>
+        <c:axId val="736057048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="90.0"/>
@@ -1187,36 +1187,55 @@
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" baseline="0">
+              <a:defRPr sz="1400" baseline="0">
                 <a:latin typeface="+mj-lt"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="677462872"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="735665432"/>
+        <c:crossesAt val="0.0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="677462872"/>
+        <c:axId val="735665432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="62.0"/>
+          <c:max val="70.0"/>
           <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1241,23 +1260,32 @@
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200">
+              <a:defRPr sz="1400">
                 <a:latin typeface="+mj-lt"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="588486440"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="736057048"/>
+        <c:crossesAt val="0.0"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="2.0"/>
       </c:valAx>
@@ -1666,7 +1694,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="R29" sqref="R29"/>
+      <selection activeCell="R35" sqref="R35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>